<commit_message>
Updated on 28th Aug 2018
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="154">
   <si>
     <t>S.NO</t>
   </si>
@@ -61,9 +61,6 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>ROUTER SIM NO.</t>
-  </si>
-  <si>
     <t>PAYMENT STATUS</t>
   </si>
   <si>
@@ -86,12 +83,593 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>Raghu</t>
+  </si>
+  <si>
+    <t>P.Venkatampalli</t>
+  </si>
+  <si>
+    <t>KLD</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>SMKR0000076</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ramasubbaiah</t>
+  </si>
+  <si>
+    <t>Chandracharla</t>
+  </si>
+  <si>
+    <t>SMKR0000078</t>
+  </si>
+  <si>
+    <t>JioFi2_0E53B6</t>
+  </si>
+  <si>
+    <t>rd6jkpsctz</t>
+  </si>
+  <si>
+    <t>5000/-</t>
+  </si>
+  <si>
+    <t>1000/-</t>
+  </si>
+  <si>
+    <t>Rakesh</t>
+  </si>
+  <si>
+    <t>Nayanavaripalli</t>
+  </si>
+  <si>
+    <t>O.D.C</t>
+  </si>
+  <si>
+    <t>SMKR0000070</t>
+  </si>
+  <si>
+    <t>JioFi2_18A739</t>
+  </si>
+  <si>
+    <t>g26ebusim9</t>
+  </si>
+  <si>
+    <t>5500/-</t>
+  </si>
+  <si>
+    <t>Jayaramulu</t>
+  </si>
+  <si>
+    <t>Kusumarupalli</t>
+  </si>
+  <si>
+    <t>SMKR0000074</t>
+  </si>
+  <si>
+    <t>JioFi2_1E4A68</t>
+  </si>
+  <si>
+    <t>656u57ejxa</t>
+  </si>
+  <si>
+    <t>LakshmiNarayana</t>
+  </si>
+  <si>
+    <t>Thumucherla</t>
+  </si>
+  <si>
+    <t>SMKR0000083</t>
+  </si>
+  <si>
+    <t>ROUTER SIM NO./Expiry</t>
+  </si>
+  <si>
+    <r>
+      <t>6300793712/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10-09-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6281559724/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20-08-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6300754020/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24-08-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6281663820/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>13-09-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6300741130/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16-09-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Durgaprasad</t>
+  </si>
+  <si>
+    <t>Nayanakota</t>
+  </si>
+  <si>
+    <t>smkr0000067</t>
+  </si>
+  <si>
+    <r>
+      <t>6301894955/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>15-09-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Bayapareddy</t>
+  </si>
+  <si>
+    <t>Ammavaripalli</t>
+  </si>
+  <si>
+    <t>PNK</t>
+  </si>
+  <si>
+    <t>smkr0000032</t>
+  </si>
+  <si>
+    <t>JioFi2_1C7596</t>
+  </si>
+  <si>
+    <t>ugx5dc5rhx</t>
+  </si>
+  <si>
+    <t>reddy</t>
+  </si>
+  <si>
+    <r>
+      <t>6300017269/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30-08-18</t>
+    </r>
+  </si>
+  <si>
+    <t>2000/-</t>
+  </si>
+  <si>
+    <t>They only recharging their router sim.</t>
+  </si>
+  <si>
+    <t>AGU/MDKS</t>
+  </si>
+  <si>
+    <t>Madakasira</t>
+  </si>
+  <si>
+    <t>MDKS</t>
+  </si>
+  <si>
+    <t>smkr0000054</t>
+  </si>
+  <si>
+    <t>JioFi2_1DFAA2</t>
+  </si>
+  <si>
+    <t>pf5gum6e39</t>
+  </si>
+  <si>
+    <t>caemdks</t>
+  </si>
+  <si>
+    <t>6300590291/-</t>
+  </si>
+  <si>
+    <t>Jayakumar</t>
+  </si>
+  <si>
+    <t>Guttur</t>
+  </si>
+  <si>
+    <t>smkr0000056</t>
+  </si>
+  <si>
+    <t>2500/-</t>
+  </si>
+  <si>
+    <t>Sadananda Reddy</t>
+  </si>
+  <si>
+    <t>Thagarakunta</t>
+  </si>
+  <si>
+    <t>smkr0000069</t>
+  </si>
+  <si>
+    <t>JioFi2_0F164C</t>
+  </si>
+  <si>
+    <t>pyzcijdt2b</t>
+  </si>
+  <si>
+    <r>
+      <t>6281964136/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>27-08-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Srinivasulu</t>
+  </si>
+  <si>
+    <t>Mithunawada</t>
+  </si>
+  <si>
+    <t>Singanamala</t>
+  </si>
+  <si>
+    <t>smkr0000061</t>
+  </si>
+  <si>
+    <t>seenu</t>
+  </si>
+  <si>
+    <r>
+      <t>6301481376/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>13-08-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Udaysekhar</t>
+  </si>
+  <si>
+    <t>Kokkanti Cross</t>
+  </si>
+  <si>
+    <t>smkr0000057</t>
+  </si>
+  <si>
+    <t>JioFi2_186794</t>
+  </si>
+  <si>
+    <t>dh9tb98rp9</t>
+  </si>
+  <si>
+    <t>Diwakar</t>
+  </si>
+  <si>
+    <t>smkr0000058</t>
+  </si>
+  <si>
+    <r>
+      <t>6301539729/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06-08-18</t>
+    </r>
+  </si>
+  <si>
+    <t>ramesh</t>
+  </si>
+  <si>
+    <t>smkr0000059</t>
+  </si>
+  <si>
+    <t>JioFi2_188878</t>
+  </si>
+  <si>
+    <t>jfprf49733</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Penubolu</t>
+  </si>
+  <si>
+    <t>C.K Palli</t>
+  </si>
+  <si>
+    <r>
+      <t>6301618682/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>05-08-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Balachandra</t>
+  </si>
+  <si>
+    <t>Podaralla</t>
+  </si>
+  <si>
+    <t>smkr0000038</t>
+  </si>
+  <si>
+    <t>JioFi3_9FAD59</t>
+  </si>
+  <si>
+    <t>66dmhw0yrr</t>
+  </si>
+  <si>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>3000/-</t>
+  </si>
+  <si>
+    <t>One year plan</t>
+  </si>
+  <si>
+    <t>Gokul</t>
+  </si>
+  <si>
+    <t>Tharimela</t>
+  </si>
+  <si>
+    <t>smkr0000062</t>
+  </si>
+  <si>
+    <t>JioFi2_0E95C8</t>
+  </si>
+  <si>
+    <t>dnzb52s74y</t>
+  </si>
+  <si>
+    <r>
+      <t>6300706152/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25-07-18</t>
+    </r>
+  </si>
+  <si>
+    <t>DhanunjayRao</t>
+  </si>
+  <si>
+    <t>Malakuntlapalli</t>
+  </si>
+  <si>
+    <t>smkr0000053</t>
+  </si>
+  <si>
+    <t>JioFi2_189AEF</t>
+  </si>
+  <si>
+    <t>t9cace5bxc</t>
+  </si>
+  <si>
+    <r>
+      <t>6300779503/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12-07-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Nagendra</t>
+  </si>
+  <si>
+    <t>smkr0000048</t>
+  </si>
+  <si>
+    <r>
+      <t>6300779733/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>02-05-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Venugopal</t>
+  </si>
+  <si>
+    <t>Salakamcheruvu</t>
+  </si>
+  <si>
+    <t>smkr0000037</t>
+  </si>
+  <si>
+    <t>JioFi2_1885BA</t>
+  </si>
+  <si>
+    <t>gmt5yf5xnz</t>
+  </si>
+  <si>
+    <t>6301462451/-</t>
+  </si>
+  <si>
+    <t>Basker Reddy</t>
+  </si>
+  <si>
+    <t>P.C Revu</t>
+  </si>
+  <si>
+    <t>MDG</t>
+  </si>
+  <si>
+    <t>smkr0000033</t>
+  </si>
+  <si>
+    <t>JioFi2_1EED9D</t>
+  </si>
+  <si>
+    <t>4ajdbkknjq</t>
+  </si>
+  <si>
+    <t>Beside Silpa</t>
+  </si>
+  <si>
+    <t>Chandra</t>
+  </si>
+  <si>
+    <t>SMKR0000079</t>
+  </si>
+  <si>
+    <t>Kuntimaddi</t>
+  </si>
+  <si>
+    <t>Jangamreddypeta</t>
+  </si>
+  <si>
+    <t>Mallikarjuna</t>
+  </si>
+  <si>
+    <t>Srinath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -161,15 +739,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -182,6 +754,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -496,16 +1084,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="10" style="8" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
@@ -515,91 +1103,1292 @@
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" customWidth="1"/>
     <col min="19" max="19" width="19" customWidth="1"/>
     <col min="20" max="20" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:20" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="3" customFormat="1">
+      <c r="B2" s="7"/>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1">
-      <c r="H2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>43326</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>43326</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="1">
+        <v>9441912299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>43330</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="1">
+        <v>9959757515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>43330</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" s="1">
+        <v>9441565119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="1" customFormat="1">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43332</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" s="1">
+        <v>9182274792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="1" customFormat="1">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
+        <v>43330</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="1">
+        <v>9959816503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="1" customFormat="1">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>43285</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="1">
+        <v>9989484837</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="1" customFormat="1">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
+        <v>43284</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="1">
+        <v>8332095555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="1" customFormat="1">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6">
+        <v>43285</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N12" s="1">
+        <v>6301368971</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" s="1">
+        <v>8328052306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="1" customFormat="1">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6">
+        <v>43315</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="1">
+        <v>9866811840</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="1" customFormat="1">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6">
+        <v>43298</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" s="1">
+        <v>7019668607</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="1" customFormat="1">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6">
+        <v>43290</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1234</v>
+      </c>
+      <c r="S15" s="1">
+        <v>8985589895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="1" customFormat="1">
+      <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6">
+        <v>43292</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" s="1">
+        <v>8885335350</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="1" customFormat="1">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6">
+        <v>43292</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="1">
+        <v>7981470083</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="1" customFormat="1">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6">
+        <v>43185</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18" s="1">
+        <v>9963771575</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="1" customFormat="1">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>43279</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L19" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="1">
+        <v>8328184014</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="1" customFormat="1">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6">
+        <v>43266</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L20" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S20" s="1">
+        <v>6300322908</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="1" customFormat="1">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6">
+        <v>43197</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="1">
+        <v>9849823290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="1" customFormat="1">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6">
+        <v>43181</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L22" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" s="1">
+        <v>9100888083</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="1" customFormat="1">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6">
+        <v>43175</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L23" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1234</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S23" s="1">
+        <v>8074457418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="1" customFormat="1">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="6">
+        <v>43325</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="1">
+        <v>12345</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1234</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S24" s="1">
+        <v>9550949721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="1" customFormat="1">
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="1" customFormat="1">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -608,7 +2397,7 @@
     <mergeCell ref="O1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Modified on 28th Aug 2018 2:02pm
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="155">
   <si>
     <t>S.NO</t>
   </si>
@@ -662,6 +662,9 @@
   <si>
     <t>Srinath</t>
   </si>
+  <si>
+    <t>To Return</t>
+  </si>
 </sst>
 </file>
 
@@ -670,7 +673,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,8 +697,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,6 +736,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA693F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -739,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -763,6 +785,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,6 +795,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -780,8 +826,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC2F04"/>
       <color rgb="FFF91B3B"/>
-      <color rgb="FFCC2F04"/>
+      <color rgb="FFA693F7"/>
+      <color rgb="FFFFFFFF"/>
     </mruColors>
   </colors>
 </styleSheet>
@@ -1084,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1108,7 +1156,7 @@
     <col min="20" max="20" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1">
+    <row r="1" spans="1:27" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1130,14 +1178,14 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="10"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1147,20 +1195,24 @@
       <c r="N1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
       <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="3" customFormat="1">
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="3" customFormat="1">
       <c r="B2" s="7"/>
       <c r="H2" s="3" t="s">
         <v>7</v>
@@ -1186,288 +1238,295 @@
       <c r="R2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" s="1" customFormat="1">
-      <c r="A4" s="1">
+      <c r="AA3" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="16" customFormat="1">
+      <c r="A4" s="16">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="19">
         <v>43326</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="H4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="16">
         <v>12345</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="16">
         <v>1234</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="1" customFormat="1">
-      <c r="A5" s="1">
+      <c r="O4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="16" customFormat="1">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="19">
         <v>43326</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="H5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="16">
         <v>12345</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="16">
         <v>1234</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="1">
+      <c r="R5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="16">
         <v>9441912299</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1">
-      <c r="A6" s="1">
+    <row r="6" spans="1:27" s="16" customFormat="1">
+      <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="19">
         <v>43330</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="H6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="16">
         <v>12345</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="16">
         <v>1234</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S6" s="1">
+      <c r="P6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S6" s="16">
         <v>9959757515</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1">
-      <c r="A7" s="1">
+    <row r="7" spans="1:27" s="16" customFormat="1">
+      <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="19">
         <v>43330</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="H7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="16">
         <v>12345</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="16">
         <v>1234</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S7" s="1">
+      <c r="O7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" s="16">
         <v>9441565119</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1">
-      <c r="A8" s="1">
+    <row r="8" spans="1:27" s="16" customFormat="1">
+      <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="19">
         <v>43332</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="H8" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="16">
         <v>12345</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="16">
         <v>1234</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S8" s="1">
+      <c r="P8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" s="16">
         <v>9182274792</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1">
+    <row r="9" spans="1:27" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1520,7 +1579,7 @@
         <v>9959816503</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1">
+    <row r="10" spans="1:27" s="1" customFormat="1">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1582,7 +1641,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="1" customFormat="1">
+    <row r="11" spans="1:27" s="1" customFormat="1">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1641,7 +1700,7 @@
         <v>8332095555</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="1" customFormat="1">
+    <row r="12" spans="1:27" s="1" customFormat="1">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1688,7 +1747,7 @@
         <v>8328052306</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="1" customFormat="1">
+    <row r="13" spans="1:27" s="1" customFormat="1">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1747,60 +1806,60 @@
         <v>9866811840</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="1" customFormat="1">
-      <c r="A14" s="1">
+    <row r="14" spans="1:27" s="13" customFormat="1">
+      <c r="A14" s="13">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="18">
         <v>43298</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="H14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="13">
         <v>1234</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N14" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S14" s="1">
+      <c r="O14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" s="13">
         <v>7019668607</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="1" customFormat="1">
+    <row r="15" spans="1:27" s="1" customFormat="1">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1844,7 +1903,7 @@
         <v>8985589895</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="1" customFormat="1">
+    <row r="16" spans="1:27" s="1" customFormat="1">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -2136,56 +2195,56 @@
         <v>6300322908</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="1" customFormat="1">
-      <c r="A21" s="1">
+    <row r="21" spans="1:20" s="13" customFormat="1">
+      <c r="A21" s="13">
         <v>18</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="18">
         <v>43197</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" s="1">
+      <c r="H21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="13">
         <v>12345</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="13">
         <v>1234</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="N21" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S21" s="1">
+      <c r="O21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="13">
         <v>9849823290</v>
       </c>
     </row>
@@ -2248,109 +2307,109 @@
         <v>9100888083</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="1" customFormat="1">
-      <c r="A23" s="1">
+    <row r="23" spans="1:20" s="13" customFormat="1">
+      <c r="A23" s="13">
         <v>20</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="18">
         <v>43175</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="H23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="13">
         <v>12345</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="13">
         <v>1234</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S23" s="1">
+      <c r="O23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S23" s="13">
         <v>8074457418</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="1" customFormat="1">
-      <c r="A24" s="1">
+    <row r="24" spans="1:20" s="16" customFormat="1">
+      <c r="A24" s="16">
         <v>21</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="19">
         <v>43325</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" s="1">
+      <c r="H24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="16">
         <v>12345</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M24" s="16">
         <v>1234</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S24" s="1">
+      <c r="O24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="S24" s="16">
         <v>9550949721</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated on 30th Aug 2018
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="161">
   <si>
     <t>S.NO</t>
   </si>
@@ -664,6 +664,37 @@
   </si>
   <si>
     <t>To Return</t>
+  </si>
+  <si>
+    <t>Veerendra</t>
+  </si>
+  <si>
+    <t>Sanapa</t>
+  </si>
+  <si>
+    <t>SMKR0000085</t>
+  </si>
+  <si>
+    <t>JioFi2_084DCB</t>
+  </si>
+  <si>
+    <t>97cjtj77yq</t>
+  </si>
+  <si>
+    <r>
+      <t>6301529835/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16-08-18</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -761,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -818,6 +849,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,10 +863,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA693F7"/>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FFCC2F04"/>
       <color rgb="FFF91B3B"/>
-      <color rgb="FFA693F7"/>
-      <color rgb="FFFFFFFF"/>
     </mruColors>
   </colors>
 </styleSheet>
@@ -1132,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2447,6 +2484,65 @@
       </c>
       <c r="F26" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" s="20" customFormat="1">
+      <c r="A27" s="20">
+        <v>24</v>
+      </c>
+      <c r="B27" s="21">
+        <v>43342</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="L27" s="20">
+        <v>12345</v>
+      </c>
+      <c r="M27" s="20">
+        <v>1234</v>
+      </c>
+      <c r="N27" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="O27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q27" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="R27" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="S27" s="20">
+        <v>9642913619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 03-09-18 10:14AM
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="166">
   <si>
     <t>S.NO</t>
   </si>
@@ -195,22 +195,6 @@
   </si>
   <si>
     <r>
-      <t>6281559724/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20-08-18</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>6300754020/</t>
     </r>
     <r>
@@ -445,22 +429,6 @@
     <t>smkr0000058</t>
   </si>
   <si>
-    <r>
-      <t>6301539729/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>06-08-18</t>
-    </r>
-  </si>
-  <si>
     <t>ramesh</t>
   </si>
   <si>
@@ -694,6 +662,79 @@
         <scheme val="minor"/>
       </rPr>
       <t>16-08-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6301368971/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>05-09-18</t>
+    </r>
+  </si>
+  <si>
+    <t>3500/-</t>
+  </si>
+  <si>
+    <r>
+      <t>6301539729/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06-08-18/28-09-18</t>
+    </r>
+  </si>
+  <si>
+    <t>JioFi2_0D74BD</t>
+  </si>
+  <si>
+    <t>jpgqiy7t49</t>
+  </si>
+  <si>
+    <r>
+      <t>Router battery expanded adapter failed,Serviced on</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 01-09-18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6281559724/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20-08-18/30-09-18</t>
     </r>
   </si>
 </sst>
@@ -840,6 +881,12 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -847,12 +894,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1171,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1190,7 +1231,7 @@
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="22.85546875" customWidth="1"/>
     <col min="19" max="19" width="19" customWidth="1"/>
-    <col min="20" max="20" width="34.42578125" customWidth="1"/>
+    <col min="20" max="20" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="3" customFormat="1">
@@ -1215,14 +1256,14 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="18"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1232,12 +1273,12 @@
       <c r="N1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
       <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1287,7 @@
       </c>
       <c r="Z1" s="11"/>
       <c r="AA1" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="3" customFormat="1">
@@ -1377,7 +1418,7 @@
         <v>1234</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>35</v>
@@ -1433,7 +1474,7 @@
         <v>1234</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>43</v>
@@ -1492,7 +1533,7 @@
         <v>1234</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O7" s="13" t="s">
         <v>29</v>
@@ -1545,7 +1586,7 @@
         <v>1234</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>43</v>
@@ -1571,10 +1612,10 @@
         <v>43330</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>39</v>
@@ -1583,7 +1624,7 @@
         <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>28</v>
@@ -1598,7 +1639,7 @@
         <v>1234</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -1624,46 +1665,46 @@
         <v>43285</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="M10" s="1">
         <v>1234</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>36</v>
@@ -1675,7 +1716,7 @@
         <v>9989484837</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:27" s="1" customFormat="1">
@@ -1686,40 +1727,40 @@
         <v>43284</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="M11" s="1">
         <v>1234</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>29</v>
@@ -1745,19 +1786,19 @@
         <v>43285</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>28</v>
@@ -1771,11 +1812,14 @@
       <c r="M12" s="1">
         <v>1234</v>
       </c>
-      <c r="N12" s="1">
-        <v>6301368971</v>
+      <c r="N12" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>28</v>
@@ -1792,10 +1836,10 @@
         <v>43315</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
@@ -1804,19 +1848,19 @@
         <v>25</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="L13" s="1">
         <v>12345</v>
@@ -1825,7 +1869,7 @@
         <v>1234</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>29</v>
@@ -1851,34 +1895,34 @@
         <v>43298</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>94</v>
       </c>
       <c r="M14" s="10">
         <v>1234</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O14" s="10" t="s">
         <v>29</v>
@@ -1904,10 +1948,10 @@
         <v>43290</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>29</v>
@@ -1916,19 +1960,19 @@
         <v>25</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="L15" s="1">
         <v>12345</v>
@@ -1948,25 +1992,31 @@
         <v>43292</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="L16" s="1">
         <v>12345</v>
@@ -1975,10 +2025,10 @@
         <v>1234</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>29</v>
@@ -1991,6 +2041,9 @@
       </c>
       <c r="S16" s="1">
         <v>8885335350</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1">
@@ -2001,10 +2054,10 @@
         <v>43292</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>29</v>
@@ -2013,28 +2066,28 @@
         <v>25</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M17" s="1">
         <v>1234</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>29</v>
@@ -2060,10 +2113,10 @@
         <v>43185</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>29</v>
@@ -2072,22 +2125,22 @@
         <v>25</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="M18" s="1">
         <v>1234</v>
@@ -2096,13 +2149,13 @@
         <v>29</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>28</v>
@@ -2111,7 +2164,7 @@
         <v>9963771575</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1">
@@ -2122,10 +2175,10 @@
         <v>43279</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
@@ -2134,19 +2187,19 @@
         <v>25</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="L19" s="1">
         <v>12345</v>
@@ -2155,7 +2208,7 @@
         <v>1234</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>29</v>
@@ -2181,10 +2234,10 @@
         <v>43266</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>29</v>
@@ -2193,19 +2246,19 @@
         <v>25</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="L20" s="1">
         <v>12345</v>
@@ -2214,7 +2267,7 @@
         <v>1234</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>29</v>
@@ -2240,10 +2293,10 @@
         <v>43197</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>29</v>
@@ -2252,7 +2305,7 @@
         <v>25</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>28</v>
@@ -2267,7 +2320,7 @@
         <v>1234</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O21" s="10" t="s">
         <v>29</v>
@@ -2293,10 +2346,10 @@
         <v>43181</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>29</v>
@@ -2305,19 +2358,19 @@
         <v>25</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="L22" s="1">
         <v>12345</v>
@@ -2326,7 +2379,7 @@
         <v>1234</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>29</v>
@@ -2352,31 +2405,31 @@
         <v>43175</v>
       </c>
       <c r="C23" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>143</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G23" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="L23" s="10">
         <v>12345</v>
@@ -2408,10 +2461,10 @@
         <v>43325</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>29</v>
@@ -2420,7 +2473,7 @@
         <v>25</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>27</v>
@@ -2456,10 +2509,10 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>29</v>
@@ -2474,10 +2527,10 @@
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>29</v>
@@ -2486,62 +2539,62 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="20" customFormat="1">
-      <c r="A27" s="20">
+    <row r="27" spans="1:20" s="17" customFormat="1">
+      <c r="A27" s="17">
         <v>24</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="18">
         <v>43342</v>
       </c>
       <c r="C27" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="H27" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="20" t="s">
+      <c r="K27" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="H27" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="20" t="s">
+      <c r="L27" s="17">
+        <v>12345</v>
+      </c>
+      <c r="M27" s="17">
+        <v>1234</v>
+      </c>
+      <c r="N27" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="K27" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="L27" s="20">
-        <v>12345</v>
-      </c>
-      <c r="M27" s="20">
-        <v>1234</v>
-      </c>
-      <c r="N27" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="O27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="R27" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="S27" s="20">
+      <c r="O27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q27" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="S27" s="17">
         <v>9642913619</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sim recharges are Updated on 03-09-18 10:41AM
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="167">
   <si>
     <t>S.NO</t>
   </si>
@@ -195,22 +195,6 @@
   </si>
   <si>
     <r>
-      <t>6300754020/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>24-08-18</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>6281663820/</t>
     </r>
     <r>
@@ -735,6 +719,25 @@
         <scheme val="minor"/>
       </rPr>
       <t>20-08-18/30-09-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Recharged on 03-09-18</t>
+  </si>
+  <si>
+    <r>
+      <t>6300754020/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24-08-18/30-09-18</t>
     </r>
   </si>
 </sst>
@@ -1212,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1287,7 +1290,7 @@
       </c>
       <c r="Z1" s="11"/>
       <c r="AA1" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="3" customFormat="1">
@@ -1418,7 +1421,7 @@
         <v>1234</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>35</v>
@@ -1431,6 +1434,9 @@
       </c>
       <c r="S5" s="13">
         <v>9441912299</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="13" customFormat="1">
@@ -1474,7 +1480,7 @@
         <v>1234</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>43</v>
@@ -1490,6 +1496,9 @@
       </c>
       <c r="S6" s="13">
         <v>9959757515</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:27" s="13" customFormat="1">
@@ -1533,7 +1542,7 @@
         <v>1234</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O7" s="13" t="s">
         <v>29</v>
@@ -1586,7 +1595,7 @@
         <v>1234</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>43</v>
@@ -1612,10 +1621,10 @@
         <v>43330</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>39</v>
@@ -1624,7 +1633,7 @@
         <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>28</v>
@@ -1639,7 +1648,7 @@
         <v>1234</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -1665,46 +1674,46 @@
         <v>43285</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="M10" s="1">
         <v>1234</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>36</v>
@@ -1716,7 +1725,7 @@
         <v>9989484837</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:27" s="1" customFormat="1">
@@ -1727,40 +1736,40 @@
         <v>43284</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="M11" s="1">
         <v>1234</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>29</v>
@@ -1786,19 +1795,19 @@
         <v>43285</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>28</v>
@@ -1813,13 +1822,13 @@
         <v>1234</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>28</v>
@@ -1836,10 +1845,10 @@
         <v>43315</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
@@ -1848,19 +1857,19 @@
         <v>25</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="L13" s="1">
         <v>12345</v>
@@ -1869,7 +1878,7 @@
         <v>1234</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>29</v>
@@ -1895,34 +1904,34 @@
         <v>43298</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="M14" s="10">
         <v>1234</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O14" s="10" t="s">
         <v>29</v>
@@ -1948,10 +1957,10 @@
         <v>43290</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>29</v>
@@ -1960,19 +1969,19 @@
         <v>25</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="L15" s="1">
         <v>12345</v>
@@ -1992,19 +2001,19 @@
         <v>43292</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>28</v>
@@ -2013,10 +2022,10 @@
         <v>27</v>
       </c>
       <c r="J16" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="L16" s="1">
         <v>12345</v>
@@ -2025,7 +2034,7 @@
         <v>1234</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>36</v>
@@ -2043,7 +2052,7 @@
         <v>8885335350</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1">
@@ -2054,10 +2063,10 @@
         <v>43292</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>29</v>
@@ -2066,28 +2075,28 @@
         <v>25</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M17" s="1">
         <v>1234</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>29</v>
@@ -2113,10 +2122,10 @@
         <v>43185</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>29</v>
@@ -2125,22 +2134,22 @@
         <v>25</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="M18" s="1">
         <v>1234</v>
@@ -2149,13 +2158,13 @@
         <v>29</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>28</v>
@@ -2164,7 +2173,7 @@
         <v>9963771575</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1">
@@ -2175,10 +2184,10 @@
         <v>43279</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
@@ -2187,19 +2196,19 @@
         <v>25</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="L19" s="1">
         <v>12345</v>
@@ -2208,7 +2217,7 @@
         <v>1234</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>29</v>
@@ -2234,10 +2243,10 @@
         <v>43266</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>29</v>
@@ -2246,19 +2255,19 @@
         <v>25</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="L20" s="1">
         <v>12345</v>
@@ -2267,7 +2276,7 @@
         <v>1234</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>29</v>
@@ -2293,10 +2302,10 @@
         <v>43197</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>29</v>
@@ -2305,7 +2314,7 @@
         <v>25</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>28</v>
@@ -2320,7 +2329,7 @@
         <v>1234</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O21" s="10" t="s">
         <v>29</v>
@@ -2346,10 +2355,10 @@
         <v>43181</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>29</v>
@@ -2358,19 +2367,19 @@
         <v>25</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="L22" s="1">
         <v>12345</v>
@@ -2379,7 +2388,7 @@
         <v>1234</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>29</v>
@@ -2405,31 +2414,31 @@
         <v>43175</v>
       </c>
       <c r="C23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G23" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23" s="10" t="s">
+      <c r="K23" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>144</v>
       </c>
       <c r="L23" s="10">
         <v>12345</v>
@@ -2461,10 +2470,10 @@
         <v>43325</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>29</v>
@@ -2473,7 +2482,7 @@
         <v>25</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>27</v>
@@ -2509,10 +2518,10 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>29</v>
@@ -2527,10 +2536,10 @@
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>29</v>
@@ -2547,10 +2556,10 @@
         <v>43342</v>
       </c>
       <c r="C27" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>29</v>
@@ -2559,19 +2568,19 @@
         <v>25</v>
       </c>
       <c r="G27" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="H27" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="17" t="s">
+      <c r="K27" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>157</v>
       </c>
       <c r="L27" s="17">
         <v>12345</v>
@@ -2580,7 +2589,7 @@
         <v>1234</v>
       </c>
       <c r="N27" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O27" s="17" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Two smkr board configurations are updated,which are installed in sanapa and thagarakunta respectively.07/09/18 :04:57 PM
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -4,20 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="176">
   <si>
     <t>S.NO</t>
   </si>
@@ -739,6 +736,46 @@
       </rPr>
       <t>24-08-18/30-09-18</t>
     </r>
+  </si>
+  <si>
+    <t>SMKR0000084</t>
+  </si>
+  <si>
+    <t>Irvine_I42H_3259</t>
+  </si>
+  <si>
+    <t>sanapa</t>
+  </si>
+  <si>
+    <t>Red and green leds are continuousily blinking.</t>
+  </si>
+  <si>
+    <r>
+      <t>9704328926/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>03-10-18</t>
+    </r>
+  </si>
+  <si>
+    <t>Sadhananda reddy</t>
+  </si>
+  <si>
+    <t>SMKR0000089</t>
+  </si>
+  <si>
+    <t>Irvine_I42H_3206</t>
+  </si>
+  <si>
+    <t>EXCHANGE</t>
   </si>
 </sst>
 </file>
@@ -780,7 +817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,6 +860,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -836,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -884,10 +927,16 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1201,22 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1230,11 +1267,12 @@
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" customWidth="1"/>
     <col min="19" max="19" width="19" customWidth="1"/>
     <col min="20" max="20" width="52.5703125" customWidth="1"/>
+    <col min="27" max="27" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="3" customFormat="1">
@@ -1259,14 +1297,14 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="20"/>
+      <c r="K1" s="22"/>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1276,12 +1314,12 @@
       <c r="N1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
       <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1379,6 +1417,10 @@
       <c r="R4" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="13" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="5" spans="1:27" s="13" customFormat="1">
       <c r="A5" s="13">
@@ -2555,7 +2597,7 @@
       <c r="B27" s="18">
         <v>43342</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="19" t="s">
         <v>152</v>
       </c>
       <c r="D27" s="17" t="s">
@@ -2605,6 +2647,124 @@
       </c>
       <c r="S27" s="17">
         <v>9642913619</v>
+      </c>
+      <c r="T27" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="1" customFormat="1">
+      <c r="A28" s="1">
+        <v>25</v>
+      </c>
+      <c r="B28" s="6">
+        <v>43349</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K28" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M28" s="1">
+        <v>1234</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S28" s="1">
+        <v>9642913619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="8">
+        <v>43349</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K29">
+        <v>12345678</v>
+      </c>
+      <c r="L29">
+        <v>12345</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1234</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" s="1">
+        <v>9866811840</v>
       </c>
     </row>
   </sheetData>
@@ -2616,28 +2776,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Guttur sim recharge details are updated on 120918 10:05AM
</commit_message>
<xml_diff>
--- a/SMKRBoardDetails_160818.xlsx
+++ b/SMKRBoardDetails_160818.xlsx
@@ -646,22 +646,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>6301368971/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>05-09-18</t>
-    </r>
-  </si>
-  <si>
     <t>3500/-</t>
   </si>
   <si>
@@ -776,6 +760,22 @@
   </si>
   <si>
     <t>EXCHANGE</t>
+  </si>
+  <si>
+    <r>
+      <t>6301368971/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>08-10-18</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="Z4" s="20"/>
       <c r="AA4" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="13" customFormat="1">
@@ -1463,7 +1463,7 @@
         <v>1234</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>35</v>
@@ -1478,7 +1478,7 @@
         <v>9441912299</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="13" customFormat="1">
@@ -1522,7 +1522,7 @@
         <v>1234</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>43</v>
@@ -1540,7 +1540,7 @@
         <v>9959757515</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:27" s="13" customFormat="1">
@@ -1864,13 +1864,13 @@
         <v>1234</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>81</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>28</v>
@@ -2064,10 +2064,10 @@
         <v>27</v>
       </c>
       <c r="J16" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="L16" s="1">
         <v>12345</v>
@@ -2076,7 +2076,7 @@
         <v>1234</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>36</v>
@@ -2094,7 +2094,7 @@
         <v>8885335350</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1">
@@ -2649,7 +2649,7 @@
         <v>9642913619</v>
       </c>
       <c r="T27" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="1" customFormat="1">
@@ -2672,28 +2672,28 @@
         <v>25</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="K28" s="1">
         <v>12345678</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M28" s="1">
         <v>1234</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>29</v>
@@ -2719,7 +2719,7 @@
         <v>43349</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>83</v>
@@ -2731,16 +2731,16 @@
         <v>25</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="K29">
         <v>12345678</v>

</xml_diff>